<commit_message>
Added ptox data edits
</commit_message>
<xml_diff>
--- a/analysis_2022/data_raw/DFD_SWP_cyano_data_2022.xlsx
+++ b/analysis_2022/data_raw/DFD_SWP_cyano_data_2022.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\AQNuisanceSpp_Program\Cyanotoxins\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/analysis_2022/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A220CF7-8230-4551-8419-FFE797CCC77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="291" documentId="13_ncr:1_{0A220CF7-8230-4551-8419-FFE797CCC77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F8D42AF-0631-44D7-BBD9-495A0CF594F1}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{19FFD934-4359-4BAB-B018-8B437E912FB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{19FFD934-4359-4BAB-B018-8B437E912FB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PTOX" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -280,6 +281,21 @@
   </si>
   <si>
     <t xml:space="preserve">4 filaments </t>
+  </si>
+  <si>
+    <t>UnitsperML</t>
+  </si>
+  <si>
+    <t>Microcystis</t>
+  </si>
+  <si>
+    <t>Cuspidothrix</t>
+  </si>
+  <si>
+    <t>Raphidopsis</t>
+  </si>
+  <si>
+    <t>SpeciesPresent</t>
   </si>
 </sst>
 </file>
@@ -674,26 +690,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252D9D04-835C-4187-86E3-31E8CF61FE4C}">
   <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.265625" customWidth="1"/>
-    <col min="2" max="2" width="16.1328125" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" customWidth="1"/>
-    <col min="4" max="4" width="14.796875" customWidth="1"/>
-    <col min="5" max="5" width="12.53125" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.53125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>44670</v>
       </c>
@@ -787,7 +803,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44676</v>
       </c>
@@ -819,7 +835,7 @@
       <c r="S3"/>
       <c r="T3" s="9"/>
     </row>
-    <row r="4" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>44676</v>
       </c>
@@ -851,7 +867,7 @@
       <c r="S4"/>
       <c r="T4" s="9"/>
     </row>
-    <row r="5" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>44676</v>
       </c>
@@ -885,7 +901,7 @@
       <c r="S5"/>
       <c r="T5" s="9"/>
     </row>
-    <row r="6" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>44698</v>
       </c>
@@ -917,7 +933,7 @@
       <c r="S6"/>
       <c r="T6" s="9"/>
     </row>
-    <row r="7" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>44704</v>
       </c>
@@ -949,7 +965,7 @@
       <c r="S7"/>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>44704</v>
       </c>
@@ -983,7 +999,7 @@
       <c r="S8"/>
       <c r="T8" s="9"/>
     </row>
-    <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>44704</v>
       </c>
@@ -1023,7 +1039,7 @@
       <c r="S9"/>
       <c r="T9" s="9"/>
     </row>
-    <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>44718</v>
       </c>
@@ -1055,7 +1071,7 @@
       <c r="S10"/>
       <c r="T10" s="9"/>
     </row>
-    <row r="11" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>44718</v>
       </c>
@@ -1091,7 +1107,7 @@
       <c r="S11"/>
       <c r="T11" s="9"/>
     </row>
-    <row r="12" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>44718</v>
       </c>
@@ -1123,7 +1139,7 @@
       <c r="S12"/>
       <c r="T12" s="9"/>
     </row>
-    <row r="13" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>44726</v>
       </c>
@@ -1161,7 +1177,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>44726</v>
       </c>
@@ -1199,7 +1215,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>44732</v>
       </c>
@@ -1233,7 +1249,7 @@
       <c r="S15"/>
       <c r="T15" s="9"/>
     </row>
-    <row r="16" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>44732</v>
       </c>
@@ -1277,7 +1293,7 @@
       <c r="S16"/>
       <c r="T16" s="9"/>
     </row>
-    <row r="17" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>44732</v>
       </c>
@@ -1311,7 +1327,7 @@
       <c r="S17"/>
       <c r="T17" s="9"/>
     </row>
-    <row r="18" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>44753</v>
       </c>
@@ -1345,7 +1361,7 @@
       <c r="S18"/>
       <c r="T18" s="9"/>
     </row>
-    <row r="19" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>44753</v>
       </c>
@@ -1387,7 +1403,7 @@
       <c r="S19"/>
       <c r="T19" s="9"/>
     </row>
-    <row r="20" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>44753</v>
       </c>
@@ -1421,7 +1437,7 @@
       <c r="S20"/>
       <c r="T20" s="9"/>
     </row>
-    <row r="21" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>44762</v>
       </c>
@@ -1455,7 +1471,7 @@
       <c r="S21"/>
       <c r="T21" s="9"/>
     </row>
-    <row r="22" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>44767</v>
       </c>
@@ -1489,7 +1505,7 @@
       <c r="S22"/>
       <c r="T22" s="9"/>
     </row>
-    <row r="23" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>44767</v>
       </c>
@@ -1533,7 +1549,7 @@
       <c r="S23"/>
       <c r="T23" s="9"/>
     </row>
-    <row r="24" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>44767</v>
       </c>
@@ -1577,7 +1593,7 @@
       <c r="S24"/>
       <c r="T24" s="9"/>
     </row>
-    <row r="25" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>44767</v>
       </c>
@@ -1621,7 +1637,7 @@
       <c r="S25"/>
       <c r="T25" s="9"/>
     </row>
-    <row r="26" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>44767</v>
       </c>
@@ -1665,7 +1681,7 @@
       <c r="S26"/>
       <c r="T26" s="9"/>
     </row>
-    <row r="27" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>44767</v>
       </c>
@@ -1703,7 +1719,7 @@
       <c r="S27"/>
       <c r="T27" s="9"/>
     </row>
-    <row r="28" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>44774</v>
       </c>
@@ -1732,7 +1748,7 @@
       <c r="S28"/>
       <c r="T28" s="9"/>
     </row>
-    <row r="29" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>44781</v>
       </c>
@@ -1776,7 +1792,7 @@
       <c r="S29"/>
       <c r="T29" s="9"/>
     </row>
-    <row r="30" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>44781</v>
       </c>
@@ -1820,7 +1836,7 @@
       <c r="S30"/>
       <c r="T30" s="9"/>
     </row>
-    <row r="31" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>44781</v>
       </c>
@@ -1864,7 +1880,7 @@
       <c r="S31"/>
       <c r="T31" s="9"/>
     </row>
-    <row r="32" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>44781</v>
       </c>
@@ -1908,7 +1924,7 @@
       <c r="S32"/>
       <c r="T32" s="9"/>
     </row>
-    <row r="33" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>44781</v>
       </c>
@@ -1952,7 +1968,7 @@
       <c r="S33"/>
       <c r="T33" s="9"/>
     </row>
-    <row r="34" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>44781</v>
       </c>
@@ -1996,7 +2012,7 @@
       <c r="S34"/>
       <c r="T34" s="9"/>
     </row>
-    <row r="35" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>44781</v>
       </c>
@@ -2040,7 +2056,7 @@
       <c r="S35"/>
       <c r="T35" s="9"/>
     </row>
-    <row r="36" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>44781</v>
       </c>
@@ -2084,7 +2100,7 @@
       <c r="S36"/>
       <c r="T36" s="9"/>
     </row>
-    <row r="37" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>44781</v>
       </c>
@@ -2132,7 +2148,7 @@
       <c r="S37"/>
       <c r="T37" s="9"/>
     </row>
-    <row r="38" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>44781</v>
       </c>
@@ -2180,7 +2196,7 @@
       <c r="S38"/>
       <c r="T38" s="9"/>
     </row>
-    <row r="39" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>44781</v>
       </c>
@@ -2228,7 +2244,7 @@
       <c r="S39"/>
       <c r="T39" s="9"/>
     </row>
-    <row r="40" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>44781</v>
       </c>
@@ -2276,7 +2292,7 @@
       <c r="S40"/>
       <c r="T40" s="9"/>
     </row>
-    <row r="41" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>44791</v>
       </c>
@@ -2308,7 +2324,7 @@
       <c r="S41"/>
       <c r="T41" s="9"/>
     </row>
-    <row r="42" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>44789</v>
       </c>
@@ -2356,7 +2372,7 @@
       <c r="S42"/>
       <c r="T42" s="9"/>
     </row>
-    <row r="43" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>44789</v>
       </c>
@@ -2404,7 +2420,7 @@
       <c r="S43"/>
       <c r="T43" s="9"/>
     </row>
-    <row r="44" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>44789</v>
       </c>
@@ -2452,7 +2468,7 @@
       <c r="S44"/>
       <c r="T44" s="9"/>
     </row>
-    <row r="45" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>44789</v>
       </c>
@@ -2486,7 +2502,7 @@
       <c r="S45"/>
       <c r="T45" s="9"/>
     </row>
-    <row r="46" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>44789</v>
       </c>
@@ -2532,7 +2548,7 @@
       <c r="S46"/>
       <c r="T46" s="9"/>
     </row>
-    <row r="47" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>44789</v>
       </c>
@@ -2576,7 +2592,7 @@
       <c r="S47"/>
       <c r="T47" s="9"/>
     </row>
-    <row r="48" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>44789</v>
       </c>
@@ -2620,7 +2636,7 @@
       <c r="S48"/>
       <c r="T48" s="9"/>
     </row>
-    <row r="49" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>44789</v>
       </c>
@@ -2664,7 +2680,7 @@
       <c r="S49"/>
       <c r="T49" s="9"/>
     </row>
-    <row r="50" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>44795</v>
       </c>
@@ -2720,7 +2736,7 @@
       <c r="S50"/>
       <c r="T50" s="9"/>
     </row>
-    <row r="51" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>44795</v>
       </c>
@@ -2754,7 +2770,7 @@
       <c r="S51"/>
       <c r="T51" s="9"/>
     </row>
-    <row r="52" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>44795</v>
       </c>
@@ -2792,7 +2808,7 @@
       <c r="S52"/>
       <c r="T52" s="9"/>
     </row>
-    <row r="53" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>44795</v>
       </c>
@@ -2836,7 +2852,7 @@
       <c r="S53"/>
       <c r="T53" s="9"/>
     </row>
-    <row r="54" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>44802</v>
       </c>
@@ -2884,7 +2900,7 @@
       <c r="S54"/>
       <c r="T54" s="9"/>
     </row>
-    <row r="55" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>44802</v>
       </c>
@@ -2932,7 +2948,7 @@
       <c r="S55"/>
       <c r="T55" s="9"/>
     </row>
-    <row r="56" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>44802</v>
       </c>
@@ -2972,7 +2988,7 @@
       <c r="S56"/>
       <c r="T56" s="9"/>
     </row>
-    <row r="57" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>44802</v>
       </c>
@@ -3012,7 +3028,7 @@
       <c r="S57"/>
       <c r="T57" s="9"/>
     </row>
-    <row r="58" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>44802</v>
       </c>
@@ -3052,7 +3068,7 @@
       <c r="S58"/>
       <c r="T58" s="9"/>
     </row>
-    <row r="59" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>44802</v>
       </c>
@@ -3092,7 +3108,7 @@
       <c r="S59"/>
       <c r="T59" s="9"/>
     </row>
-    <row r="60" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>44802</v>
       </c>
@@ -3132,7 +3148,7 @@
       <c r="S60"/>
       <c r="T60" s="9"/>
     </row>
-    <row r="61" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>44802</v>
       </c>
@@ -3175,4 +3191,1315 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDABA237-A34F-4CE2-B995-DB31B7F989CD}">
+  <dimension ref="A1:E76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>44670</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>44676</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>44676</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>44676</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>44698</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>44704</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>44704</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>44704</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>44704</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>44718</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>44718</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>44718</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>44726</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="10">
+        <v>4</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>44726</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="10">
+        <v>2</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>44732</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="10">
+        <v>3</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>44732</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="10">
+        <v>4</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>44732</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>44732</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="10">
+        <v>4</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>44732</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="10">
+        <v>2</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>44753</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>44753</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>44753</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>44753</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="10">
+        <v>20</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>44753</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="10">
+        <v>3</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>44762</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>44767</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>44767</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="10">
+        <v>2</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>44767</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="10">
+        <v>30</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>44767</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="10">
+        <v>20</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>44767</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="10">
+        <v>10</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>44767</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="10">
+        <v>3</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>44774</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>44781</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>44781</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="10">
+        <v>4</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>44781</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="10">
+        <v>100</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>44781</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="10">
+        <v>3</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>44781</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="10">
+        <v>2</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>44783</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="10">
+        <v>4</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>44781</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="10">
+        <v>150</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
+        <v>44781</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="10">
+        <v>5</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>44783</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="10">
+        <v>5</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>44783</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
+        <v>44791</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="10">
+        <v>75</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="10">
+        <v>80</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="10">
+        <v>100</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="10">
+        <v>20</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="10">
+        <v>4</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="10">
+        <v>5</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="10">
+        <v>30</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="10">
+        <v>3</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="10">
+        <v>10</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="10">
+        <v>5</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
+        <v>44789</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="10">
+        <v>10</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="10">
+        <v>700</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" s="10">
+        <v>40</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="10">
+        <v>4</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="10">
+        <v>4</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" s="10">
+        <v>3</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" s="10">
+        <v>3</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64" s="10">
+        <v>5</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" s="10">
+        <v>1</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="10">
+        <v>50</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D67" s="10">
+        <v>12</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="8">
+        <v>44795</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" s="10">
+        <v>1</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="8">
+        <v>44802</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D69" s="10">
+        <v>200</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="8">
+        <v>44802</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" s="10">
+        <v>100</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="8">
+        <v>44802</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" s="10">
+        <v>5</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="8">
+        <v>44802</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="10">
+        <v>2</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="8">
+        <v>44802</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D73" s="10">
+        <v>1</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="8">
+        <v>44802</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="10">
+        <v>2</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="8">
+        <v>44802</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" s="10">
+        <v>5</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="8">
+        <v>44802</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D76" s="10">
+        <v>4</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>